<commit_message>
add apd dan aps
</commit_message>
<xml_diff>
--- a/apd.xlsx
+++ b/apd.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="629">
   <si>
     <t>Program Studi</t>
   </si>
@@ -2061,15 +2061,9 @@
     <t>KEGIATAN DOSEN TETAP DALAM SEMINAR DLL</t>
   </si>
   <si>
-    <t>DONE</t>
-  </si>
-  <si>
     <t>REFERENCE 3.1.1</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>referensi ke 3A 4.3.1</t>
   </si>
   <si>
@@ -2089,6 +2083,39 @@
   </si>
   <si>
     <t>refer ke 3A 6.2.3</t>
+  </si>
+  <si>
+    <t>Inputan Manual dari user</t>
+  </si>
+  <si>
+    <t>Inputan manual dari user</t>
+  </si>
+  <si>
+    <t>Hanya edit data karena add data nya sudah oleh admin</t>
+  </si>
+  <si>
+    <t>Select data ke table dosen</t>
+  </si>
+  <si>
+    <t>Kaprodi, Admin</t>
+  </si>
+  <si>
+    <t>Kaprodi, Admin, Akademik</t>
+  </si>
+  <si>
+    <t>Kaprodi, Admin, Student Tracer</t>
+  </si>
+  <si>
+    <t>Kaprodi, Admin, Keuangan</t>
+  </si>
+  <si>
+    <t>Kaprodi, Admin, General Affair</t>
+  </si>
+  <si>
+    <t>Kaprodi, Admin, Kepala Perpus</t>
+  </si>
+  <si>
+    <t>Dekan, Kaprodi, Admin, Keuangan</t>
   </si>
 </sst>
 </file>
@@ -13109,13 +13136,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="37.5" style="5" customWidth="1"/>
     <col min="2" max="2" width="9.375" style="5" customWidth="1"/>
     <col min="3" max="3" width="11.625" style="62" customWidth="1"/>
     <col min="4" max="4" width="96.5" style="5" customWidth="1"/>
@@ -13133,25 +13160,43 @@
     </row>
     <row r="6" spans="1:5" ht="11.1" customHeight="1"/>
     <row r="7" spans="1:5">
+      <c r="A7" s="5" t="s">
+        <v>622</v>
+      </c>
       <c r="B7" s="147"/>
       <c r="C7" s="241"/>
       <c r="D7" s="142" t="s">
         <v>362</v>
       </c>
+      <c r="E7" s="5" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
+      <c r="A8" s="5" t="s">
+        <v>622</v>
+      </c>
       <c r="B8" s="148"/>
       <c r="C8" s="242"/>
       <c r="D8" s="143" t="s">
         <v>245</v>
       </c>
+      <c r="E8" s="5" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
+      <c r="A9" s="5" t="s">
+        <v>622</v>
+      </c>
       <c r="B9" s="149"/>
       <c r="C9" s="243"/>
       <c r="D9" s="144" t="s">
         <v>246</v>
       </c>
+      <c r="E9" s="5" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="B10" s="179" t="s">
@@ -13166,7 +13211,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
-        <v>610</v>
+        <v>623</v>
       </c>
       <c r="B11" s="244" t="s">
         <v>449</v>
@@ -13180,7 +13225,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="5" t="s">
-        <v>610</v>
+        <v>623</v>
       </c>
       <c r="B12" s="245" t="s">
         <v>449</v>
@@ -13194,7 +13239,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>610</v>
+        <v>623</v>
       </c>
       <c r="B13" s="245" t="s">
         <v>449</v>
@@ -13208,7 +13253,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>612</v>
+        <v>624</v>
       </c>
       <c r="B14" s="245" t="s">
         <v>449</v>
@@ -13227,7 +13272,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B16" s="245" t="s">
         <v>449</v>
@@ -13241,7 +13286,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B17" s="245" t="s">
         <v>449</v>
@@ -13255,7 +13300,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B18" s="245" t="s">
         <v>449</v>
@@ -13269,7 +13314,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B19" s="245" t="s">
         <v>449</v>
@@ -13283,7 +13328,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B20" s="245" t="s">
         <v>449</v>
@@ -13297,7 +13342,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B21" s="245" t="s">
         <v>449</v>
@@ -13311,7 +13356,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B22" s="245" t="s">
         <v>449</v>
@@ -13325,7 +13370,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B23" s="245" t="s">
         <v>449</v>
@@ -13339,7 +13384,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B24" s="245" t="s">
         <v>449</v>
@@ -13353,7 +13398,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B25" s="245" t="s">
         <v>449</v>
@@ -13367,7 +13412,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B26" s="245" t="s">
         <v>449</v>
@@ -13381,7 +13426,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B27" s="245" t="s">
         <v>449</v>
@@ -13400,7 +13445,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B29" s="245" t="s">
         <v>449</v>
@@ -13414,7 +13459,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B30" s="245" t="s">
         <v>449</v>
@@ -13428,7 +13473,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B31" s="245" t="s">
         <v>449</v>
@@ -13442,7 +13487,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B32" s="245" t="s">
         <v>449</v>
@@ -13461,7 +13506,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="5" t="s">
-        <v>612</v>
+        <v>625</v>
       </c>
       <c r="B34" s="245" t="s">
         <v>449</v>
@@ -13475,7 +13520,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="5" t="s">
-        <v>612</v>
+        <v>625</v>
       </c>
       <c r="B35" s="245" t="s">
         <v>449</v>
@@ -13489,7 +13534,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="5" t="s">
-        <v>612</v>
+        <v>625</v>
       </c>
       <c r="B36" s="245" t="s">
         <v>449</v>
@@ -13503,7 +13548,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="5" t="s">
-        <v>612</v>
+        <v>625</v>
       </c>
       <c r="B37" s="245" t="s">
         <v>449</v>
@@ -13517,7 +13562,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="5" t="s">
-        <v>612</v>
+        <v>626</v>
       </c>
       <c r="B38" s="245" t="s">
         <v>449</v>
@@ -13531,7 +13576,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="5" t="s">
-        <v>612</v>
+        <v>627</v>
       </c>
       <c r="B39" s="245" t="s">
         <v>449</v>
@@ -13545,7 +13590,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B40" s="245" t="s">
         <v>449</v>
@@ -13564,7 +13609,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B42" s="245" t="s">
         <v>449</v>
@@ -13578,7 +13623,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B43" s="245" t="s">
         <v>449</v>
@@ -13592,7 +13637,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B44" s="245" t="s">
         <v>449</v>
@@ -13611,7 +13656,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="5" t="s">
-        <v>612</v>
+        <v>623</v>
       </c>
       <c r="B46" s="245" t="s">
         <v>455</v>
@@ -13625,7 +13670,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="5" t="s">
-        <v>612</v>
+        <v>623</v>
       </c>
       <c r="B47" s="245" t="s">
         <v>455</v>
@@ -13644,7 +13689,7 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B49" s="245" t="s">
         <v>455</v>
@@ -13656,12 +13701,12 @@
         <v>365</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B50" s="245" t="s">
         <v>455</v>
@@ -13675,7 +13720,7 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B51" s="245" t="s">
         <v>455</v>
@@ -13687,7 +13732,7 @@
         <v>476</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="12.95" customHeight="1">
@@ -13697,7 +13742,7 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="5" t="s">
-        <v>612</v>
+        <v>628</v>
       </c>
       <c r="B53" s="245" t="s">
         <v>455</v>
@@ -13709,12 +13754,12 @@
         <v>477</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="5" t="s">
-        <v>612</v>
+        <v>625</v>
       </c>
       <c r="B54" s="245" t="s">
         <v>455</v>
@@ -13726,12 +13771,12 @@
         <v>453</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="5" t="s">
-        <v>612</v>
+        <v>625</v>
       </c>
       <c r="B55" s="245" t="s">
         <v>455</v>
@@ -13745,7 +13790,7 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="5" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B56" s="245" t="s">
         <v>455</v>
@@ -13757,7 +13802,7 @@
         <v>479</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="12.95" customHeight="1">
@@ -13767,7 +13812,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="5" t="s">
-        <v>612</v>
+        <v>625</v>
       </c>
       <c r="B58" s="245" t="s">
         <v>455</v>
@@ -13779,12 +13824,12 @@
         <v>480</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="5" t="s">
-        <v>612</v>
+        <v>625</v>
       </c>
       <c r="B59" s="245" t="s">
         <v>455</v>
@@ -13796,7 +13841,7 @@
         <v>481</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="12.95" customHeight="1">
@@ -29794,8 +29839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="D1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="18.75"/>
@@ -29951,7 +29996,9 @@
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="5"/>
+      <c r="A18" s="5" t="s">
+        <v>618</v>
+      </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -46027,9 +46074,7 @@
   </sheetPr>
   <dimension ref="A3:S20"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
-    </sheetView>
+    <sheetView topLeftCell="J1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="18.75"/>
   <cols>
@@ -46450,7 +46495,7 @@
   <sheetData>
     <row r="2" spans="1:17">
       <c r="D2" s="5" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="23.1" customHeight="1"/>

</xml_diff>